<commit_message>
Enhancement: Tables and media ref are updated when inserting or removing a column. Fixed: Added missing logic and tests
</commit_message>
<xml_diff>
--- a/spec/integration/data/test-update-ref.xlsx
+++ b/spec/integration/data/test-update-ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthis.clavijo\Documents\dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17980219-E17C-4F91-8871-A4D105AD1C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E10657E-7976-4259-A09D-E8C2863C92FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22860" yWindow="0" windowWidth="14400" windowHeight="7365" activeTab="1" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,11 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet3!$E$24:$E$30</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet3!$N$27</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet3!$N$27</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Supercar</t>
   </si>
@@ -93,9 +98,6 @@
     <t>Sukhoi Su-27 Flanker</t>
   </si>
   <si>
-    <t>16 000 kg</t>
-  </si>
-  <si>
     <t>Mach 2.35</t>
   </si>
   <si>
@@ -268,6 +270,12 @@
   </si>
   <si>
     <t>Latest Release</t>
+  </si>
+  <si>
+    <t>16 000 kg</t>
+  </si>
+  <si>
+    <t>Rating</t>
   </si>
 </sst>
 </file>
@@ -317,17 +325,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -338,6 +354,857 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Most liked distro</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$C$24:$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Linux Mint</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Endeavour OS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MX Linux</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Manjaro Linux</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fedora</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Pop!_OS</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Ubuntu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$24:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5A2A-4AE9-8BCB-463CCA008718}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="1848740896"/>
+        <c:axId val="1848744640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1848740896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1848744640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1848744640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1848740896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -351,9 +1218,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2584</xdr:colOff>
+      <xdr:colOff>293077</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>149087</xdr:rowOff>
+      <xdr:rowOff>142737</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -382,8 +1249,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1311826" y="2090392"/>
-          <a:ext cx="1755323" cy="1520825"/>
+          <a:off x="1302269" y="2100905"/>
+          <a:ext cx="2031481" cy="1522120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -445,15 +1312,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>198782</xdr:colOff>
+      <xdr:colOff>201957</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>82827</xdr:rowOff>
+      <xdr:rowOff>86002</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
+      <xdr:colOff>432288</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>160079</xdr:rowOff>
+      <xdr:rowOff>163254</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -482,14 +1349,55 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3263347" y="7007088"/>
-          <a:ext cx="2440194" cy="2452428"/>
+          <a:off x="3242630" y="7046579"/>
+          <a:ext cx="2662870" cy="2458502"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>59871</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161018</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24A98C5F-96E0-A25C-6FA0-F414F16B5189}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -520,6 +1428,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E6DC6A24-64E0-496C-8D25-19FAFAE8D248}" name="Table47" displayName="Table47" ref="C23:E30" totalsRowShown="0">
+  <autoFilter ref="C23:E30" xr:uid="{E6DC6A24-64E0-496C-8D25-19FAFAE8D248}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C24:E30">
+    <sortCondition descending="1" ref="E23:E30"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8CE279F9-E9FC-408F-8270-91248CD19603}" name="Linux Distro"/>
+    <tableColumn id="2" xr3:uid="{3AA04AFC-CD95-4818-AF4C-A467DC36C108}" name="Latest Release"/>
+    <tableColumn id="3" xr3:uid="{DC098437-B7C5-442A-B99A-71998A688431}" name="Rating" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{96066BCA-1793-49C6-9398-26BE9511A5E4}" name="Table3" displayName="Table3" ref="A1:B27" totalsRowShown="0">
   <autoFilter ref="A1:B27" xr:uid="{96066BCA-1793-49C6-9398-26BE9511A5E4}"/>
   <tableColumns count="2">
@@ -530,12 +1453,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BDC05BB0-1D10-4ACC-9F63-5419CB5795F5}" name="Table4" displayName="Table4" ref="F8:G15" totalsRowShown="0">
-  <autoFilter ref="F8:G15" xr:uid="{BDC05BB0-1D10-4ACC-9F63-5419CB5795F5}"/>
-  <tableColumns count="2">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BDC05BB0-1D10-4ACC-9F63-5419CB5795F5}" name="Table4" displayName="Table4" ref="F8:H15" totalsRowShown="0">
+  <autoFilter ref="F8:H15" xr:uid="{BDC05BB0-1D10-4ACC-9F63-5419CB5795F5}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F4D73304-6EE1-4F2C-A84A-B30CDEE18311}" name="Linux Distro"/>
     <tableColumn id="2" xr3:uid="{9B036167-052A-4ECB-847B-9ED77ACF1651}" name="Latest Release"/>
+    <tableColumn id="3" xr3:uid="{A8647AD9-BCE9-4BED-962A-771FD14B403C}" name="Rating" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -841,7 +1765,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -934,59 +1858,59 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -997,35 +1921,35 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
         <v>39</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1042,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A22E23F-ACE4-46FC-8EBF-965A4BA4AAE6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1055,22 +1979,121 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DB8D49-655F-472E-A309-10E2A26D5997}">
-  <dimension ref="A1"/>
+  <dimension ref="C23:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="2">
+        <v>44640</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8.7100000000000009</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2">
+        <v>44737</v>
+      </c>
+      <c r="E25" s="3">
+        <v>8.65</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="2">
+        <v>44661</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="2">
+        <v>44731</v>
+      </c>
+      <c r="E27" s="3">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="2">
+        <v>44691</v>
+      </c>
+      <c r="E28" s="3">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="2">
+        <v>44676</v>
+      </c>
+      <c r="E29" s="3">
+        <v>8.2200000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="2">
+        <v>44672</v>
+      </c>
+      <c r="E30" s="3">
+        <v>7.6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E6487E-2723-47F2-A993-0FBBC51B7B51}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="F8" sqref="F8:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,182 +2102,207 @@
     <col min="2" max="2" width="18.81640625" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="2">
         <v>44661</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="3">
+        <v>8.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2">
         <v>44737</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="3">
+        <v>8.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2">
         <v>44640</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="3">
+        <v>8.7100000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2">
         <v>44731</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="3">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G13" s="2">
         <v>44676</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="3">
+        <v>8.2200000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="2">
         <v>44672</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" s="3">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="2">
         <v>44691</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" s="3">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1262,7 +2310,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1270,7 +2318,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1278,7 +2326,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1286,7 +2334,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1294,7 +2342,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1302,7 +2350,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1310,7 +2358,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1318,7 +2366,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1326,7 +2374,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1334,7 +2382,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1342,14 +2390,15 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>